<commit_message>
adding lists code + exp
</commit_message>
<xml_diff>
--- a/experiment_code/Jsontest.xlsx
+++ b/experiment_code/Jsontest.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bowdoin-my.sharepoint.com/personal/rwarburt_bowdoin_edu/Documents/School/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhilashakumar/fluency-switch-experiment/experiment_code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="8_{8182C57B-ED3D-FF41-9C44-723BF1D857BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7AD84B88-99F4-2D4B-B871-5C228420E16E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B924380-FE50-FA46-B12D-185FB1206F2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15800" activeTab="1" xr2:uid="{2CE71DE1-AEE8-7B47-8ED4-876E0822E198}"/>
+    <workbookView xWindow="380" yWindow="760" windowWidth="28040" windowHeight="15800" xr2:uid="{2CE71DE1-AEE8-7B47-8ED4-876E0822E198}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="53">
   <si>
     <t>Subject</t>
   </si>
@@ -190,6 +190,12 @@
   </si>
   <si>
     <t>hello, goodbye</t>
+  </si>
+  <si>
+    <t>domain</t>
+  </si>
+  <si>
+    <t>animals</t>
   </si>
 </sst>
 </file>
@@ -549,388 +555,529 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D76CDF7-5C27-5B4D-A1F9-E02328D988A7}">
-  <dimension ref="A1:B47"/>
+  <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>51</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>51</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>51</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>51</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>51</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>51</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>51</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>51</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>51</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>51</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>51</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>51</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>51</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>51</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>51</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>51</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>51</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>51</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>51</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>51</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>51</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>51</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>51</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C24" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>51</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C25" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>51</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C26" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>51</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>51</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C28" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>51</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>10</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C30" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>10</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C31" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>10</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C32" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>10</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C33" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>10</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C34" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>10</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C35" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>10</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C36" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>78</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C37" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>78</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C38" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>78</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C39" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>78</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C40" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>78</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C41" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>78</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C42" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>78</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C43" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>78</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C44" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>78</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C45" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>78</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C46" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>78</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>47</v>
+      </c>
+      <c r="C47" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -942,7 +1089,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B86073E-514E-354F-9D0C-9842179FA5BB}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>

</xml_diff>